<commit_message>
Fixing returns and testUnknown
</commit_message>
<xml_diff>
--- a/Results /21 April 2020.xlsx
+++ b/Results /21 April 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Results /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6F47D3-ADE9-1047-8EA6-2E5FF0DF37C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50400980-82A0-804E-85A4-17F952880A70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>Negative DES</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>Accuracy Score =  accuracy_score(y_test, y_pred)</t>
+  </si>
+  <si>
+    <t>DES2017</t>
+  </si>
+  <si>
+    <t>Std</t>
+  </si>
+  <si>
+    <t>Jacobs</t>
+  </si>
+  <si>
+    <t>DES2017 + Jacobs</t>
   </si>
 </sst>
 </file>
@@ -258,7 +270,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -612,6 +624,47 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -620,23 +673,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -646,15 +693,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -664,54 +702,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
@@ -720,14 +721,73 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1042,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06CD785-33B7-3045-A313-C2EB4D15E3B6}">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:AE29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1053,34 +1113,36 @@
     <col min="1" max="1" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" style="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="10.83203125" style="54"/>
-    <col min="17" max="17" width="10.83203125" style="23"/>
-    <col min="18" max="18" width="26.33203125" style="54" customWidth="1"/>
-    <col min="19" max="19" width="35.33203125" style="54" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="2"/>
+    <col min="13" max="13" width="12.1640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="10.83203125" style="36"/>
+    <col min="17" max="17" width="10.83203125" style="18"/>
+    <col min="18" max="18" width="26.33203125" style="36" customWidth="1"/>
+    <col min="19" max="19" width="35.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="10.83203125" style="18"/>
+    <col min="23" max="23" width="10.83203125" style="36"/>
+    <col min="24" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="3"/>
@@ -1092,17 +1154,20 @@
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-    </row>
-    <row r="2" spans="1:20" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="37" t="s">
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="35"/>
+    </row>
+    <row r="2" spans="1:31" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="52"/>
+      <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="28" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="3"/>
@@ -1114,19 +1179,18 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-    </row>
-    <row r="3" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+    </row>
+    <row r="3" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="26" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="3"/>
@@ -1138,17 +1202,16 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-    </row>
-    <row r="4" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40" t="s">
+    </row>
+    <row r="4" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="53"/>
+      <c r="B4" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="30" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="3"/>
@@ -1160,17 +1223,16 @@
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-    </row>
-    <row r="5" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
-      <c r="B5" s="37" t="s">
+    </row>
+    <row r="5" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="54"/>
+      <c r="B5" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="28" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="3"/>
@@ -1182,228 +1244,295 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-    </row>
-    <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+    </row>
+    <row r="6" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="G6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="55"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
-    </row>
-    <row r="7" spans="1:20" s="24" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="64"/>
+    </row>
+    <row r="7" spans="1:31" s="19" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="9" t="s">
+      <c r="E7" s="45"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="43" t="s">
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="44"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="59" t="s">
+      <c r="K7" s="48"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="60" t="s">
+      <c r="N7" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="60" t="s">
+      <c r="O7" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="60" t="s">
+      <c r="P7" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" s="61" t="s">
+      <c r="Q7" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="R7" s="62" t="s">
+      <c r="R7" s="43" t="s">
         <v>46</v>
       </c>
       <c r="S7" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="T7" s="45"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="27">
+      <c r="T7" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="65"/>
+      <c r="X7" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="48"/>
+      <c r="AA7" s="65"/>
+      <c r="AB7" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC7" s="48"/>
+      <c r="AD7" s="48"/>
+      <c r="AE7" s="65"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" s="56">
         <v>1</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="17" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="50" t="s">
+      <c r="E8" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="52" t="s">
+      <c r="H8" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="52" t="s">
+      <c r="I8" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="51" t="s">
+      <c r="J8" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="52" t="s">
+      <c r="K8" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="L8" s="52" t="s">
+      <c r="L8" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="M8" s="51" t="s">
+      <c r="M8" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="N8" s="58" t="s">
+      <c r="N8" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="O8" s="58" t="s">
+      <c r="O8" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="58" t="s">
+      <c r="P8" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="Q8" s="51" t="s">
+      <c r="Q8" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="R8" s="53"/>
-      <c r="S8" s="53"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="22" t="s">
+      <c r="R8" s="35"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="U8" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="V8" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="X8" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y8" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z8" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA8" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB8" s="66" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC8" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD8" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE8" s="67" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A9" s="57"/>
+      <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
-      <c r="B10" s="22" t="s">
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A10" s="57"/>
+      <c r="B10" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="22" t="s">
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A11" s="57"/>
+      <c r="B11" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30" t="s">
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A12" s="58"/>
+      <c r="B12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="56"/>
-      <c r="O12" s="56"/>
-      <c r="P12" s="56"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="56"/>
-      <c r="S12" s="56"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="38"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A14" s="55"/>
+      <c r="B14" s="55"/>
     </row>
     <row r="21" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="6"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="6"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="6"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="6"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="6"/>
+      <c r="C29" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="AB7:AE7"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="X7:AA7"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A8:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1420,37 +1549,37 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Removing excess print statements
</commit_message>
<xml_diff>
--- a/Results /21 April 2020.xlsx
+++ b/Results /21 April 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/Results /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50400980-82A0-804E-85A4-17F952880A70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11F970F-14DD-1B4D-8BEF-BC3F6AC4A2D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{EE8A5D69-8514-D648-BD1F-175D6DB078D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -629,42 +629,40 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -673,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -713,6 +711,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
@@ -782,12 +781,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1102,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06CD785-33B7-3045-A313-C2EB4D15E3B6}">
-  <dimension ref="A1:AE29"/>
+  <dimension ref="A1:AF29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1123,17 +1124,17 @@
     <col min="11" max="11" width="5.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="10.83203125" style="36"/>
+    <col min="14" max="16" width="10.83203125" style="37"/>
     <col min="17" max="17" width="10.83203125" style="18"/>
-    <col min="18" max="18" width="26.33203125" style="36" customWidth="1"/>
+    <col min="18" max="18" width="26.33203125" style="37" customWidth="1"/>
     <col min="19" max="19" width="35.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="10.83203125" style="18"/>
-    <col min="23" max="23" width="10.83203125" style="36"/>
-    <col min="24" max="16384" width="10.83203125" style="2"/>
+    <col min="20" max="30" width="10.83203125" style="18"/>
+    <col min="31" max="31" width="10.83203125" style="37"/>
+    <col min="32" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:32" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="52" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="25" t="s">
@@ -1154,13 +1155,22 @@
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="35"/>
-    </row>
-    <row r="2" spans="1:31" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+    </row>
+    <row r="2" spans="1:32" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53"/>
       <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
@@ -1179,9 +1189,22 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
-    </row>
-    <row r="3" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51" t="s">
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+    </row>
+    <row r="3" spans="1:32" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="52" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="25" t="s">
@@ -1202,9 +1225,22 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
-    </row>
-    <row r="4" spans="1:31" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="53"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+    </row>
+    <row r="4" spans="1:32" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="54"/>
       <c r="B4" s="29" t="s">
         <v>11</v>
       </c>
@@ -1223,9 +1259,22 @@
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
-    </row>
-    <row r="5" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+    </row>
+    <row r="5" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="55"/>
       <c r="B5" s="27" t="s">
         <v>14</v>
       </c>
@@ -1244,25 +1293,50 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
-    </row>
-    <row r="6" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+    </row>
+    <row r="6" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="G6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="64"/>
-    </row>
-    <row r="7" spans="1:31" s="19" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="38"/>
+      <c r="AB6" s="38"/>
+      <c r="AC6" s="38"/>
+      <c r="AD6" s="38"/>
+      <c r="AE6" s="38"/>
+      <c r="AF6" s="38"/>
+    </row>
+    <row r="7" spans="1:32" s="19" customFormat="1" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>29</v>
       </c>
@@ -1272,63 +1346,64 @@
       <c r="C7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="47" t="s">
+      <c r="E7" s="46"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="49" t="s">
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="48"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="40" t="s">
+      <c r="K7" s="49"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="41" t="s">
+      <c r="N7" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="41" t="s">
+      <c r="O7" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="41" t="s">
+      <c r="P7" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" s="42" t="s">
+      <c r="Q7" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="R7" s="43" t="s">
+      <c r="R7" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="S7" s="62" t="s">
+      <c r="S7" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="T7" s="47" t="s">
+      <c r="T7" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="U7" s="48"/>
-      <c r="V7" s="48"/>
-      <c r="W7" s="65"/>
-      <c r="X7" s="47" t="s">
+      <c r="U7" s="51"/>
+      <c r="V7" s="51"/>
+      <c r="W7" s="68"/>
+      <c r="X7" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="Y7" s="48"/>
-      <c r="Z7" s="48"/>
-      <c r="AA7" s="65"/>
-      <c r="AB7" s="47" t="s">
+      <c r="Y7" s="51"/>
+      <c r="Z7" s="51"/>
+      <c r="AA7" s="68"/>
+      <c r="AB7" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="AC7" s="48"/>
-      <c r="AD7" s="48"/>
-      <c r="AE7" s="65"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A8" s="56">
+      <c r="AC7" s="51"/>
+      <c r="AD7" s="51"/>
+      <c r="AE7" s="68"/>
+      <c r="AF7" s="31"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A8" s="57">
         <v>1</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -1337,120 +1412,114 @@
       <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="J8" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="N8" s="39" t="s">
+      <c r="N8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="O8" s="39" t="s">
+      <c r="O8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="39" t="s">
+      <c r="P8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="Q8" s="33" t="s">
+      <c r="Q8" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="R8" s="35"/>
-      <c r="S8" s="63"/>
-      <c r="T8" s="66" t="s">
+      <c r="R8" s="36"/>
+      <c r="S8" s="64"/>
+      <c r="T8" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="U8" s="66" t="s">
+      <c r="U8" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="V8" s="66" t="s">
+      <c r="V8" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="W8" s="67" t="s">
+      <c r="W8" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="X8" s="66" t="s">
+      <c r="X8" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="Y8" s="66" t="s">
+      <c r="Y8" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="Z8" s="66" t="s">
+      <c r="Z8" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="AA8" s="67" t="s">
+      <c r="AA8" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AB8" s="66" t="s">
+      <c r="AB8" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="AC8" s="66" t="s">
+      <c r="AC8" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="AD8" s="66" t="s">
+      <c r="AD8" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="AE8" s="67" t="s">
+      <c r="AE8" s="66" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A9" s="57"/>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A9" s="58"/>
       <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A10" s="57"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A10" s="58"/>
       <c r="B10" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A11" s="57"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A11" s="58"/>
       <c r="B11" s="17" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A12" s="58"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A12" s="59"/>
       <c r="B12" s="22" t="s">
         <v>22</v>
       </c>
@@ -1465,25 +1534,31 @@
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="24"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
       <c r="Q12" s="24"/>
-      <c r="R12" s="38"/>
+      <c r="R12" s="39"/>
       <c r="S12" s="24"/>
       <c r="T12" s="24"/>
       <c r="U12" s="24"/>
       <c r="V12" s="24"/>
-      <c r="W12" s="38"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="24"/>
+      <c r="AA12" s="24"/>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="24"/>
+      <c r="AD12" s="24"/>
+      <c r="AE12" s="39"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A14" s="55"/>
-      <c r="B14" s="55"/>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A14" s="56"/>
+      <c r="B14" s="56"/>
     </row>
     <row r="21" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1575,11 +1650,11 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>